<commit_message>
initial support for coffeescript (but it needs to move to cv)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="11055"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -360,7 +361,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -393,9 +396,21 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<script xmlns="http://tempuri.org/inject/script">
-  <source><![CDATA[
+<script xmlns="http://tempuri.org/inject/script" version="1.1">
+  <source version="1.1" language="CoffeeScript"><![CDATA[
 var ws = Application.ActiveWorkbook.Sheets.Add();
 ws.SelectionChange = function(){
 	console.log( Application.ActiveCell.Address());

</xml_diff>

<commit_message>
Starting multi-window support (Excel15)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="11055"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -361,7 +362,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,6 +372,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -384,18 +399,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -408,9 +411,21 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <script xmlns="http://tempuri.org/inject/script" version="1.1">
-  <source version="1.1" language="CoffeeScript"><![CDATA[
+  <source version="1.1" language="Javascript"><![CDATA[
 var ws = Application.ActiveWorkbook.Sheets.Add();
 ws.SelectionChange = function(){
 	console.log( Application.ActiveCell.Address());

</xml_diff>

<commit_message>
initial cut at prefs/customization
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,11 +12,7 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="11055"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -362,7 +358,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,64 +367,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <script xmlns="http://tempuri.org/inject/script" version="1.1">
   <source version="1.1" language="Javascript"><![CDATA[
 var ws = Application.ActiveWorkbook.Sheets.Add();
 ws.SelectionChange = function(){
-	console.log( Application.ActiveCell.Address());
+	console.log( Application.Selection.Address());
 };
 ]]></source>
 </script>

</xml_diff>